<commit_message>
Regen titres/domaines + lexique + antconc request
Regen les titres par domaines
Regen le lexique du corpus
Utilisé le fichier dans Antconc pour produire un fichier de résultat
retravaillé sous Excel pour la requête :
</commit_message>
<xml_diff>
--- a/results/titres_par_domaines.xlsx
+++ b/results/titres_par_domaines.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19226"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19330"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\damie_000\Documents\GitHub\tal\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B05A62AF-13C8-4F6D-B598-BDCF06EF44C9}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95916247-1510-4A14-99A8-72709A3C1A8F}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7695" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1308" uniqueCount="1303">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1309" uniqueCount="1304">
   <si>
     <t>0.shs</t>
   </si>
@@ -3942,6 +3942,9 @@
   </si>
   <si>
     <t>Est-ce que le domaine a des sous-domaines ?</t>
+  </si>
+  <si>
+    <t>En vert, les domaines de 0.info</t>
   </si>
 </sst>
 </file>
@@ -4058,28 +4061,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Pourcentage" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="10">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="7">
     <dxf>
       <fill>
         <patternFill>
@@ -4097,7 +4079,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="9"/>
+          <bgColor theme="6"/>
         </patternFill>
       </fill>
     </dxf>
@@ -4168,8 +4150,8 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{7B85C980-5211-443C-ADFC-7CEEA00ACA11}" name="domain__1" displayName="domain__1" ref="A1:E394" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="A1:E394" xr:uid="{58DB4BF9-2082-4E13-8487-13B4EEB77205}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{C26ED54D-F618-42FA-BA0E-1C9E2F466AAA}" uniqueName="1" name="code_s" queryTableFieldId="1" dataDxfId="9"/>
-    <tableColumn id="2" xr3:uid="{E1BB39C9-2E05-44E4-B907-F49088C7739E}" uniqueName="2" name="label_s" queryTableFieldId="2" dataDxfId="8"/>
+    <tableColumn id="1" xr3:uid="{C26ED54D-F618-42FA-BA0E-1C9E2F466AAA}" uniqueName="1" name="code_s" queryTableFieldId="1" dataDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{E1BB39C9-2E05-44E4-B907-F49088C7739E}" uniqueName="2" name="label_s" queryTableFieldId="2" dataDxfId="5"/>
     <tableColumn id="3" xr3:uid="{AC1A1636-6F2C-40EF-A767-E01B6A04AAFE}" uniqueName="3" name="level_i" queryTableFieldId="3"/>
     <tableColumn id="4" xr3:uid="{1C582498-955D-4AAF-A6B3-C51BE825E061}" uniqueName="4" name="parent_i" queryTableFieldId="4"/>
     <tableColumn id="6" xr3:uid="{39C4D1CA-4925-45CE-8521-6F87CB9355BD}" uniqueName="6" name="haveNext_bool" queryTableFieldId="6"/>
@@ -4465,7 +4447,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D488"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A184" workbookViewId="0">
       <selection activeCell="D71" sqref="D71"/>
     </sheetView>
   </sheetViews>
@@ -9946,22 +9928,22 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1">
-    <cfRule type="containsText" dxfId="7" priority="4" operator="containsText" text=".sdv">
+    <cfRule type="containsText" dxfId="4" priority="4" operator="containsText" text=".sdv">
       <formula>NOT(ISERROR(SEARCH(".sdv",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="5" operator="containsText" text=".shs">
+    <cfRule type="containsText" dxfId="3" priority="5" operator="containsText" text=".shs">
       <formula>NOT(ISERROR(SEARCH(".shs",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text=".shs.">
-      <formula>NOT(ISERROR(SEARCH(".shs.",A1)))</formula>
+    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text=".info.">
+      <formula>NOT(ISERROR(SEARCH(".info.",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="2" operator="containsText" text=".sdv.">
+    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text=".sdv.">
       <formula>NOT(ISERROR(SEARCH(".sdv.",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text=".info.">
-      <formula>NOT(ISERROR(SEARCH(".info.",A1)))</formula>
+    <cfRule type="containsText" dxfId="0" priority="3" operator="containsText" text=".shs.">
+      <formula>NOT(ISERROR(SEARCH(".shs.",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -9973,10 +9955,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A8975B6-F98B-42F2-A063-CCF8C2ACA632}">
-  <dimension ref="A1:D25"/>
+  <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10077,97 +10059,104 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="9"/>
+      <c r="C13" s="11" t="s">
+        <v>1303</v>
+      </c>
       <c r="D13" s="9"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="9"/>
-      <c r="B14" s="9"/>
-      <c r="C14" s="10" t="s">
-        <v>1297</v>
-      </c>
       <c r="D14" s="9"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="9"/>
+      <c r="B15" s="9"/>
+      <c r="C15" s="10" t="s">
+        <v>1297</v>
+      </c>
       <c r="D15" s="9"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="9"/>
-      <c r="B16" s="4" t="s">
-        <v>505</v>
-      </c>
-      <c r="C16" t="s">
-        <v>1298</v>
-      </c>
       <c r="D16" s="9"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="9"/>
       <c r="B17" s="4" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="C17" t="s">
-        <v>1299</v>
+        <v>1298</v>
       </c>
       <c r="D17" s="9"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="9"/>
       <c r="B18" s="4" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="C18" t="s">
-        <v>1300</v>
+        <v>1299</v>
       </c>
       <c r="D18" s="9"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="9"/>
       <c r="B19" s="4" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="C19" t="s">
-        <v>1301</v>
+        <v>1300</v>
       </c>
       <c r="D19" s="9"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="9"/>
       <c r="B20" s="4" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="C20" t="s">
-        <v>1302</v>
+        <v>1301</v>
       </c>
       <c r="D20" s="9"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="9"/>
+      <c r="B21" s="4" t="s">
+        <v>509</v>
+      </c>
+      <c r="C21" t="s">
+        <v>1302</v>
+      </c>
       <c r="D21" s="9"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="9"/>
-      <c r="C22" t="s">
-        <v>503</v>
-      </c>
       <c r="D22" s="9"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="9"/>
-      <c r="C23" s="7" t="s">
-        <v>504</v>
+      <c r="C23" t="s">
+        <v>503</v>
       </c>
       <c r="D23" s="9"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="9"/>
+      <c r="C24" s="7" t="s">
+        <v>504</v>
+      </c>
       <c r="D24" s="9"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="9"/>
-      <c r="B25" s="9"/>
-      <c r="C25" s="9"/>
       <c r="D25" s="9"/>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="9"/>
+      <c r="B26" s="9"/>
+      <c r="C26" s="9"/>
+      <c r="D26" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>